<commit_message>
Ajout de l'Organigramme du projet
</commit_message>
<xml_diff>
--- a/Doc/Tache.xlsx
+++ b/Doc/Tache.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="27">
   <si>
     <t>Exécuté par</t>
   </si>
@@ -527,8 +527,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I175"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -708,7 +708,9 @@
       <c r="D10" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="E10" s="6"/>
+      <c r="E10" s="6" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="11" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="10" t="s">
@@ -723,7 +725,9 @@
       <c r="D11" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="E11" s="6"/>
+      <c r="E11" s="6" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="12" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
@@ -738,7 +742,9 @@
       <c r="D12" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="E12" s="6"/>
+      <c r="E12" s="6" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="13" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="10" t="s">

</xml_diff>

<commit_message>
Update de Denise pour le 14/11/14
</commit_message>
<xml_diff>
--- a/Doc/Tache.xlsx
+++ b/Doc/Tache.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="28">
   <si>
     <t>Exécuté par</t>
   </si>
@@ -97,6 +97,9 @@
   </si>
   <si>
     <t>ok</t>
+  </si>
+  <si>
+    <t>FlStudio (gratuit en version d'essai pour faire de la musique), recherches de tutoriaux/exemple de compo jv</t>
   </si>
 </sst>
 </file>
@@ -527,8 +530,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I175"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -693,7 +696,9 @@
       <c r="D9" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="E9" s="6"/>
+      <c r="E9" s="6" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="10" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">

</xml_diff>

<commit_message>
Nouvelles organisation, taches et format txt
</commit_message>
<xml_diff>
--- a/Doc/Tache.xlsx
+++ b/Doc/Tache.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="46">
   <si>
     <t>Exécuté par</t>
   </si>
@@ -99,14 +99,68 @@
     <t>ok</t>
   </si>
   <si>
-    <t>FlStudio (gratuit en version d'essai pour faire de la musique), recherches de tutoriaux/exemple de compo jv</t>
+    <t>Création d'une interface de jeu + Menu principale</t>
+  </si>
+  <si>
+    <t>1 musique = 4jours a 1 semaine</t>
+  </si>
+  <si>
+    <t>5 sons par jour</t>
+  </si>
+  <si>
+    <t>Création du premier sprite (Personnage qui marche vers la droite =&gt; 10 IMAGES environ)</t>
+  </si>
+  <si>
+    <t>Création de 10 mécanismes (Pieges) différents</t>
+  </si>
+  <si>
+    <t>Problème de compréhension dans la tache : Réponse pas assé précises,</t>
+  </si>
+  <si>
+    <t>&lt;-----&gt;</t>
+  </si>
+  <si>
+    <t>&lt;----------&gt;</t>
+  </si>
+  <si>
+    <t>Création de la premiere musique d'ambience : menu principal</t>
+  </si>
+  <si>
+    <t>Renseignement sur les prés-requis pour la création d'une start-up</t>
+  </si>
+  <si>
+    <t>Liste des différentes action possible par le joueur / personnage</t>
+  </si>
+  <si>
+    <t>Création des premiers décors de monde                                                         (Voir suivie Design/decor/ 1 à 10)</t>
+  </si>
+  <si>
+    <t>Création du premier fond                                                                                        (Voir suivie Design/fond/monde1)</t>
+  </si>
+  <si>
+    <t>Semaine du 17/11/2014 au 24/11/2014</t>
+  </si>
+  <si>
+    <t>Semaine du 25/11/2014 au 1/12/2014</t>
+  </si>
+  <si>
+    <t>Recrutement : 2 Graphistes + 1 Sound désigner</t>
+  </si>
+  <si>
+    <t>Organisation de la réunion 0.1 et rédaction du fichier "Reunion.txt" Expliquant le but le déroulement des réunion (Fréquence de 1 réunion toute les 2 semaines)</t>
+  </si>
+  <si>
+    <t>création des premiers sons                                                                         (Voir suivie Design/sons/ 1 à 5)</t>
+  </si>
+  <si>
+    <t>Correction orthographes / syntaxe de la totalité du Repo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -142,6 +196,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -151,7 +212,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -174,11 +235,96 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -226,6 +372,86 @@
     <xf numFmtId="14" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -530,8 +756,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I175"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -602,7 +828,14 @@
       <c r="D3" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="8"/>
+      <c r="E3" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="G3" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="H3" s="16"/>
+      <c r="I3" s="16"/>
     </row>
     <row r="4" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
@@ -618,6 +851,12 @@
         <v>8</v>
       </c>
       <c r="E4" s="8"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="H4" s="16"/>
+      <c r="I4" s="16"/>
     </row>
     <row r="5" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
@@ -633,6 +872,10 @@
         <v>8</v>
       </c>
       <c r="E5" s="8"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="16"/>
+      <c r="I5" s="16"/>
     </row>
     <row r="6" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
@@ -648,6 +891,10 @@
         <v>8</v>
       </c>
       <c r="E6" s="6"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="16"/>
+      <c r="I6" s="16"/>
     </row>
     <row r="7" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="13" t="s">
@@ -665,6 +912,10 @@
       <c r="E7" s="6" t="s">
         <v>26</v>
       </c>
+      <c r="F7" s="16"/>
+      <c r="G7" s="16"/>
+      <c r="H7" s="16"/>
+      <c r="I7" s="16"/>
     </row>
     <row r="8" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="13" t="s">
@@ -696,9 +947,7 @@
       <c r="D9" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="E9" s="6" t="s">
-        <v>27</v>
-      </c>
+      <c r="E9" s="6"/>
     </row>
     <row r="10" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
@@ -752,7 +1001,7 @@
       </c>
     </row>
     <row r="13" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="10" t="s">
+      <c r="A13" s="17" t="s">
         <v>8</v>
       </c>
       <c r="B13" s="10" t="s">
@@ -767,102 +1016,218 @@
       <c r="E13" s="6"/>
     </row>
     <row r="14" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="6"/>
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
+      <c r="A14" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="E14" s="30" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="15" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="6"/>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
+      <c r="A15" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="9">
+        <v>41961</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>8</v>
+      </c>
       <c r="E15" s="6"/>
     </row>
     <row r="16" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="6"/>
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
+      <c r="A16" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" s="20">
+        <v>41962</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>8</v>
+      </c>
       <c r="E16" s="6"/>
     </row>
     <row r="17" spans="1:5" ht="75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="6"/>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
+      <c r="A17" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" s="32" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17" s="20">
+        <v>41963</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>8</v>
+      </c>
       <c r="E17" s="6"/>
     </row>
     <row r="18" spans="1:5" ht="75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="6"/>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
+      <c r="A18" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="C18" s="14">
+        <v>41961</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>8</v>
+      </c>
       <c r="E18" s="6"/>
     </row>
     <row r="19" spans="1:5" ht="75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="6"/>
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
+      <c r="A19" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="C19" s="33">
+        <v>41967</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>8</v>
+      </c>
       <c r="E19" s="6"/>
     </row>
     <row r="20" spans="1:5" ht="75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="6"/>
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
+      <c r="A20" s="37" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" s="37" t="s">
+        <v>45</v>
+      </c>
+      <c r="C20" s="33">
+        <v>41967</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E20" s="23"/>
     </row>
     <row r="21" spans="1:5" ht="75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="6"/>
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
+      <c r="A21" s="34" t="s">
+        <v>17</v>
+      </c>
+      <c r="B21" s="35" t="s">
+        <v>39</v>
+      </c>
+      <c r="C21" s="27">
+        <v>41960</v>
+      </c>
+      <c r="D21" s="36" t="s">
+        <v>8</v>
+      </c>
+      <c r="E21" s="22"/>
     </row>
     <row r="22" spans="1:5" ht="75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="6"/>
-      <c r="B22" s="6"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
+      <c r="A22" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C22" s="27">
+        <v>41961</v>
+      </c>
+      <c r="D22" s="10" t="s">
+        <v>8</v>
+      </c>
       <c r="E22" s="6"/>
     </row>
     <row r="23" spans="1:5" ht="75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="6"/>
-      <c r="B23" s="6"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
+      <c r="A23" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B23" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="C23" s="27">
+        <v>41967</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>8</v>
+      </c>
       <c r="E23" s="6"/>
     </row>
     <row r="24" spans="1:5" ht="75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="6"/>
-      <c r="B24" s="6"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="6"/>
+      <c r="A24" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C24" s="29">
+        <v>41961</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>8</v>
+      </c>
       <c r="E24" s="6"/>
     </row>
     <row r="25" spans="1:5" ht="75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="6"/>
-      <c r="B25" s="6"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
+      <c r="A25" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="C25" s="29">
+        <v>41967</v>
+      </c>
+      <c r="D25" s="10" t="s">
+        <v>8</v>
+      </c>
       <c r="E25" s="6"/>
     </row>
     <row r="26" spans="1:5" ht="75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="6"/>
-      <c r="B26" s="6"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="6"/>
+      <c r="A26" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C26" s="29">
+        <v>41967</v>
+      </c>
+      <c r="D26" s="10" t="s">
+        <v>8</v>
+      </c>
       <c r="E26" s="6"/>
     </row>
     <row r="27" spans="1:5" ht="75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="6"/>
-      <c r="B27" s="6"/>
-      <c r="C27" s="6"/>
-      <c r="D27" s="6"/>
-      <c r="E27" s="6"/>
+      <c r="A27" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="B27" s="31" t="s">
+        <v>41</v>
+      </c>
+      <c r="C27" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="D27" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="E27" s="30" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="28" spans="1:5" ht="75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="6"/>

</xml_diff>

<commit_message>
Mise a jour des tâches
</commit_message>
<xml_diff>
--- a/Doc/Tache.xlsx
+++ b/Doc/Tache.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="49">
   <si>
     <t>Exécuté par</t>
   </si>
@@ -157,6 +157,12 @@
   </si>
   <si>
     <t>Fl studio, première approche, visionnage d'exemple de compo, reaper installation</t>
+  </si>
+  <si>
+    <t>Le cahier des charge sera a refaire et a voir avec jaime. Non fait</t>
+  </si>
+  <si>
+    <t>Reporté au 17/11/2014 pour raison d'indisponibilité le week end du 15 au 16 novembre 2014. Joyeux anniversaire !</t>
   </si>
 </sst>
 </file>
@@ -759,8 +765,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I175"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -874,7 +880,9 @@
       <c r="D5" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="8"/>
+      <c r="E5" s="10" t="s">
+        <v>48</v>
+      </c>
       <c r="F5" s="16"/>
       <c r="G5" s="16"/>
       <c r="H5" s="16"/>
@@ -950,7 +958,7 @@
       <c r="D9" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="E9" s="6" t="s">
+      <c r="E9" s="13" t="s">
         <v>46</v>
       </c>
     </row>
@@ -1018,7 +1026,9 @@
       <c r="D13" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="E13" s="6"/>
+      <c r="E13" s="10" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="14" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="30" t="s">

</xml_diff>

<commit_message>
MaJ Taches et recrutement
</commit_message>
<xml_diff>
--- a/Doc/Tache.xlsx
+++ b/Doc/Tache.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="51">
   <si>
     <t>Exécuté par</t>
   </si>
@@ -163,6 +163,12 @@
   </si>
   <si>
     <t>Reporté au 17/11/2014 pour raison d'indisponibilité le week end du 15 au 16 novembre 2014. Joyeux anniversaire !</t>
+  </si>
+  <si>
+    <t>A finir pour le 17/11/2017</t>
+  </si>
+  <si>
+    <t>Décalé au 24/11/2014</t>
   </si>
 </sst>
 </file>
@@ -765,8 +771,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I175"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -859,7 +865,9 @@
       <c r="D4" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="8"/>
+      <c r="E4" s="10" t="s">
+        <v>49</v>
+      </c>
       <c r="F4" s="16"/>
       <c r="G4" s="16" t="s">
         <v>29</v>
@@ -1060,7 +1068,9 @@
       <c r="D15" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="E15" s="6"/>
+      <c r="E15" s="10" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="16" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="19" t="s">

</xml_diff>

<commit_message>
Ajout de Nicolas dans les taches
</commit_message>
<xml_diff>
--- a/Doc/Tache.xlsx
+++ b/Doc/Tache.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="52">
   <si>
     <t>Exécuté par</t>
   </si>
@@ -169,13 +169,16 @@
   </si>
   <si>
     <t>Décalé au 24/11/2014</t>
+  </si>
+  <si>
+    <t>Nicolas</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -214,6 +217,13 @@
     <font>
       <sz val="16"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFFC000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -339,7 +349,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -468,6 +478,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -771,8 +782,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I175"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -845,6 +856,9 @@
       </c>
       <c r="E3" s="10" t="s">
         <v>32</v>
+      </c>
+      <c r="F3" s="38" t="s">
+        <v>51</v>
       </c>
       <c r="G3" s="16" t="s">
         <v>28</v>

</xml_diff>

<commit_message>
Mise à jour tâches
</commit_message>
<xml_diff>
--- a/Doc/Tache.xlsx
+++ b/Doc/Tache.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicolas\Desktop\Groom\Doc\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="72" windowWidth="22116" windowHeight="9528"/>
   </bookViews>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="53">
   <si>
     <t>Exécuté par</t>
   </si>
@@ -172,6 +177,9 @@
   </si>
   <si>
     <t>Nicolas</t>
+  </si>
+  <si>
+    <t>Correction des fautes d'orthographe</t>
   </si>
 </sst>
 </file>
@@ -349,7 +357,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -479,6 +487,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -488,6 +508,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -536,7 +559,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -571,7 +594,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -780,10 +803,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I175"/>
+  <dimension ref="A1:I176"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1252,28 +1275,36 @@
       <c r="E26" s="6"/>
     </row>
     <row r="27" spans="1:5" ht="75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="30" t="s">
+      <c r="A27" s="39" t="s">
+        <v>51</v>
+      </c>
+      <c r="B27" s="40" t="s">
+        <v>52</v>
+      </c>
+      <c r="C27" s="41">
+        <v>41967</v>
+      </c>
+      <c r="D27" s="39" t="s">
+        <v>51</v>
+      </c>
+      <c r="E27" s="6"/>
+    </row>
+    <row r="28" spans="1:5" ht="75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="B27" s="31" t="s">
+      <c r="B28" s="31" t="s">
         <v>41</v>
       </c>
-      <c r="C27" s="30" t="s">
+      <c r="C28" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="D27" s="30" t="s">
+      <c r="D28" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="E27" s="30" t="s">
+      <c r="E28" s="30" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" ht="75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="6"/>
-      <c r="B28" s="6"/>
-      <c r="C28" s="6"/>
-      <c r="D28" s="6"/>
-      <c r="E28" s="6"/>
     </row>
     <row r="29" spans="1:5" ht="75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="6"/>
@@ -2303,6 +2334,13 @@
       <c r="C175" s="6"/>
       <c r="D175" s="6"/>
       <c r="E175" s="6"/>
+    </row>
+    <row r="176" spans="1:5" ht="75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A176" s="6"/>
+      <c r="B176" s="6"/>
+      <c r="C176" s="6"/>
+      <c r="D176" s="6"/>
+      <c r="E176" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Correction + cahier des charges
Correction de l'orthographe + suppression du cahier des charges
</commit_message>
<xml_diff>
--- a/Doc/Tache.xlsx
+++ b/Doc/Tache.xlsx
@@ -21,20 +21,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="53">
   <si>
     <t>Exécuté par</t>
   </si>
   <si>
-    <t>Déscription de tâche</t>
-  </si>
-  <si>
     <t>Date de la tâche</t>
   </si>
   <si>
-    <t xml:space="preserve">Tâche donné par </t>
-  </si>
-  <si>
     <t>Problèmes rencontrés</t>
   </si>
   <si>
@@ -50,63 +44,21 @@
     <t>Alexandre</t>
   </si>
   <si>
-    <t>Noté : OK ! Si aucun problème n'est rencontré.</t>
-  </si>
-  <si>
-    <t>Rédaction d'un Background Complet donnant une ligne diréctive au projet. Quelle est la place du joueur dans le jeu, ce qu'il représente … Quel est le but du personnage, qui il est, et comment arrive t'il à ses fins</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Donner les prmiere mécanique de jeu, comment s'enchaine un "Monde" , comment le joueur intéragit avec le personnage. </t>
-  </si>
-  <si>
-    <t>Création d'un premier "Level". Mécanique complête, design complet, enchainement des évènement complet.</t>
-  </si>
-  <si>
     <t>L'heure de rendu pour chaque tâche est de 21h00</t>
   </si>
   <si>
-    <t>Personne devant éxécuter la tache</t>
-  </si>
-  <si>
-    <t>Déscription complete et présise de la tâche à éffectuer</t>
-  </si>
-  <si>
-    <t>Personne donnant la tâche à éxécuter.</t>
-  </si>
-  <si>
     <t>Céline</t>
   </si>
   <si>
-    <t>Création d'un écrant titre. Personnage complet en action avec un décord. Le tous en 1024 * 768</t>
-  </si>
-  <si>
     <t>Création d'une doc GIT (Push, importation exportation ajout)</t>
   </si>
   <si>
-    <t>Création d'un Fichier de contacte regroupant les information personnels de chacun des membre du groupe</t>
-  </si>
-  <si>
-    <t>Composition / Recherche d'une musique décrivant l'univer du jeu</t>
-  </si>
-  <si>
-    <t>Création d'un premier moteur phisique dans le jeu</t>
-  </si>
-  <si>
-    <t>Mise en place d'une architecture de travail au sein du groupe de dévelopement</t>
-  </si>
-  <si>
-    <t>Création de l'emploi du temps de travail des dévelopeur.</t>
-  </si>
-  <si>
     <t>Mise en place d'un premier cahier des charge au projet "Groom"</t>
   </si>
   <si>
     <t>ok</t>
   </si>
   <si>
-    <t>Création d'une interface de jeu + Menu principale</t>
-  </si>
-  <si>
     <t>1 musique = 4jours a 1 semaine</t>
   </si>
   <si>
@@ -116,27 +68,15 @@
     <t>Création du premier sprite (Personnage qui marche vers la droite =&gt; 10 IMAGES environ)</t>
   </si>
   <si>
-    <t>Création de 10 mécanismes (Pieges) différents</t>
-  </si>
-  <si>
-    <t>Problème de compréhension dans la tache : Réponse pas assé précises,</t>
-  </si>
-  <si>
     <t>&lt;-----&gt;</t>
   </si>
   <si>
     <t>&lt;----------&gt;</t>
   </si>
   <si>
-    <t>Création de la premiere musique d'ambience : menu principal</t>
-  </si>
-  <si>
     <t>Renseignement sur les prés-requis pour la création d'une start-up</t>
   </si>
   <si>
-    <t>Liste des différentes action possible par le joueur / personnage</t>
-  </si>
-  <si>
     <t>Création des premiers décors de monde                                                         (Voir suivie Design/decor/ 1 à 10)</t>
   </si>
   <si>
@@ -158,9 +98,6 @@
     <t>création des premiers sons                                                                         (Voir suivie Design/sons/ 1 à 5)</t>
   </si>
   <si>
-    <t>Correction orthographes / syntaxe de la totalité du Repo</t>
-  </si>
-  <si>
     <t>Fl studio, première approche, visionnage d'exemple de compo, reaper installation</t>
   </si>
   <si>
@@ -180,6 +117,69 @@
   </si>
   <si>
     <t>Correction des fautes d'orthographe</t>
+  </si>
+  <si>
+    <t>Personne devant exécuter la tâche</t>
+  </si>
+  <si>
+    <t>Description complète et précise de la tâche à effectuer</t>
+  </si>
+  <si>
+    <t>Description de tâche</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tâche donnée par </t>
+  </si>
+  <si>
+    <t>Personne donnant la tâche à exécuter.</t>
+  </si>
+  <si>
+    <t>Noter : OK ! Si aucun problème n'est rencontré.</t>
+  </si>
+  <si>
+    <t>Rédaction d'un Background Complet donnant une ligne directive au projet. Quelle est la place du joueur dans le jeu, ce qu'il représente … Quel est le but du personnage, qui il est, et comment arrive t'il à ses fins</t>
+  </si>
+  <si>
+    <t>Problème de compréhension dans la tache : Réponses pas assez précises.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Donner les premières mécaniques de jeu, comment s'enchaine un "Monde" , comment le joueur intéragit avec le personnage. </t>
+  </si>
+  <si>
+    <t>Création d'un premier "Level". Mécanique complète, design complet, enchaînement des évènements complets.</t>
+  </si>
+  <si>
+    <t>Création d'un écran titre. Personnage complet en action avec un décord. Le tous en 1024 * 768</t>
+  </si>
+  <si>
+    <t>Création d'un Fichier de contact regroupant les informations personnelles de chacun des membre du groupe</t>
+  </si>
+  <si>
+    <t>Composition / Recherche d'une musique décrivant l'univers du jeu</t>
+  </si>
+  <si>
+    <t>Création d'un premier moteur physique dans le jeu</t>
+  </si>
+  <si>
+    <t>Mise en place d'une architecture de travail au sein du groupe de développement</t>
+  </si>
+  <si>
+    <t>Création de l'emploi du temps de travail des développeurs.</t>
+  </si>
+  <si>
+    <t>Création d'une interface de jeu + Menu principal</t>
+  </si>
+  <si>
+    <t>Liste des différentes actions possibles par le joueur / personnage</t>
+  </si>
+  <si>
+    <t>Création de 10 mécanismes (Pièges) différents</t>
+  </si>
+  <si>
+    <t>Création de la première musique d'ambience : menu principal</t>
+  </si>
+  <si>
+    <t>Correction orthographe / syntaxe de la totalité du Repo</t>
   </si>
 </sst>
 </file>
@@ -805,8 +805,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I176"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -823,110 +823,110 @@
         <v>0</v>
       </c>
       <c r="B1" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="D1" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" s="7" t="s">
         <v>2</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>9</v>
+        <v>37</v>
       </c>
       <c r="F2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>7</v>
-      </c>
       <c r="I2" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>10</v>
+        <v>38</v>
       </c>
       <c r="C3" s="9">
         <v>41956</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="F3" s="38" t="s">
-        <v>51</v>
+        <v>30</v>
       </c>
       <c r="G3" s="16" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="H3" s="16"/>
       <c r="I3" s="16"/>
     </row>
     <row r="4" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="C4" s="9">
         <v>41957</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>49</v>
+        <v>28</v>
       </c>
       <c r="F4" s="16"/>
       <c r="G4" s="16" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="H4" s="16"/>
       <c r="I4" s="16"/>
     </row>
     <row r="5" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>12</v>
+        <v>41</v>
       </c>
       <c r="C5" s="9">
         <v>41959</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>48</v>
+        <v>27</v>
       </c>
       <c r="F5" s="16"/>
       <c r="G5" s="16"/>
@@ -935,16 +935,16 @@
     </row>
     <row r="6" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
       <c r="C6" s="12">
         <v>41957</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E6" s="6"/>
       <c r="F6" s="16"/>
@@ -954,19 +954,19 @@
     </row>
     <row r="7" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="13" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="C7" s="14">
         <v>41956</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="F7" s="16"/>
       <c r="G7" s="16"/>
@@ -975,335 +975,337 @@
     </row>
     <row r="8" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="13" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="C8" s="14">
         <v>41956</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="13" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="C9" s="14">
         <v>41957</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E9" s="13" t="s">
-        <v>46</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>22</v>
+        <v>45</v>
       </c>
       <c r="C10" s="15">
         <v>41955</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="10" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>23</v>
+        <v>46</v>
       </c>
       <c r="C11" s="15">
         <v>41956</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>24</v>
+        <v>47</v>
       </c>
       <c r="C12" s="15">
         <v>41955</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="17" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="C13" s="15">
         <v>41957</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>47</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="30" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="B14" s="31" t="s">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="D14" s="30" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="E14" s="30" t="s">
-        <v>34</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="21" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B15" s="18" t="s">
-        <v>27</v>
+        <v>48</v>
       </c>
       <c r="C15" s="9">
         <v>41961</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>50</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="19" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B16" s="25" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="C16" s="20">
         <v>41962</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E16" s="6"/>
     </row>
     <row r="17" spans="1:5" ht="75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="18" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B17" s="32" t="s">
-        <v>31</v>
+        <v>50</v>
       </c>
       <c r="C17" s="20">
         <v>41963</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E17" s="6"/>
     </row>
     <row r="18" spans="1:5" ht="75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="13" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>44</v>
+        <v>24</v>
       </c>
       <c r="C18" s="14">
         <v>41961</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E18" s="6"/>
     </row>
     <row r="19" spans="1:5" ht="75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="13" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B19" s="24" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="C19" s="33">
         <v>41967</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E19" s="6"/>
     </row>
     <row r="20" spans="1:5" ht="75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="37" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B20" s="37" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="C20" s="33">
         <v>41967</v>
       </c>
       <c r="D20" s="10" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E20" s="23"/>
     </row>
     <row r="21" spans="1:5" ht="75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="34" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="B21" s="35" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="C21" s="27">
         <v>41960</v>
       </c>
       <c r="D21" s="36" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E21" s="22"/>
     </row>
     <row r="22" spans="1:5" ht="75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="26" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>38</v>
+        <v>18</v>
       </c>
       <c r="C22" s="27">
         <v>41961</v>
       </c>
       <c r="D22" s="10" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E22" s="6"/>
     </row>
     <row r="23" spans="1:5" ht="75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="11" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="B23" s="28" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="C23" s="27">
         <v>41967</v>
       </c>
       <c r="D23" s="10" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E23" s="6"/>
     </row>
     <row r="24" spans="1:5" ht="75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="10" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>36</v>
+        <v>17</v>
       </c>
       <c r="C24" s="29">
         <v>41961</v>
       </c>
       <c r="D24" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="E24" s="6"/>
+        <v>6</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="25" spans="1:5" ht="75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="10" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="C25" s="29">
         <v>41967</v>
       </c>
       <c r="D25" s="10" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E25" s="6"/>
     </row>
     <row r="26" spans="1:5" ht="75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="10" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>43</v>
+        <v>23</v>
       </c>
       <c r="C26" s="29">
         <v>41967</v>
       </c>
       <c r="D26" s="10" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E26" s="6"/>
     </row>
     <row r="27" spans="1:5" ht="75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="39" t="s">
-        <v>51</v>
+        <v>30</v>
       </c>
       <c r="B27" s="40" t="s">
-        <v>52</v>
+        <v>31</v>
       </c>
       <c r="C27" s="41">
         <v>41967</v>
       </c>
       <c r="D27" s="39" t="s">
-        <v>51</v>
+        <v>30</v>
       </c>
       <c r="E27" s="6"/>
     </row>
     <row r="28" spans="1:5" ht="75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="30" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="B28" s="31" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="C28" s="30" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="D28" s="30" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="E28" s="30" t="s">
-        <v>34</v>
+        <v>16</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="75" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>